<commit_message>
previously added measurements.xlsx - added all data and charts
</commit_message>
<xml_diff>
--- a/fractals/measurements.xlsx
+++ b/fractals/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\cse3320\fractals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76328E7-878F-4E40-9F4A-5C27B5E0BDC3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460CEB48-6ACA-4024-A0D9-F23F50B0AAC7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415" xr2:uid="{E7B87478-65B0-4663-BD55-47C23FACC279}"/>
   </bookViews>
@@ -121,6 +121,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandelseries (omega)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -160,18 +185,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1:$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandelseries (omega)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution times / # processes</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -265,6 +279,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -330,6 +399,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -463,6 +591,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandel -x -.5 -y -.5 -s 1 -m 2000 -n # (omega) </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -502,18 +655,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$10:$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandel -x -.5 -y -.5 -s 1 -m 2000 -n # (omega)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution time / # threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -613,6 +755,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -678,6 +875,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -811,6 +1063,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandel -x 0.2869325 -y 0.0142905 -s .000001 -W 1024 -H 1024 -m 1000 -n # (omega)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -850,18 +1127,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$20:$B$21</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandel -x 0.2869325 -y 0.0142905 -s .000001 -W 1024 -H 1024 -m 1000 -n # (omega)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution time / # threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1081,6 +1347,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1146,6 +1467,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1279,6 +1655,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandelseries (cse3320.org)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1318,18 +1719,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$31:$B$32</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandelseries (cse3320.org)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution time / # processes</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1537,6 +1927,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1602,6 +2047,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (usec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1735,6 +2240,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandel -x -.5 -y -.5 -s 1 -m 2000 -n # (cse3320.org)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1774,18 +2304,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$40:$B$41</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandel -x -.5 -y -.5 -s 1 -m 2000 -n # (cse3320.org)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution time / # threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2005,6 +2524,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2070,6 +2644,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2203,6 +2832,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>mandel -x 0.2869325 -y 0.0142905 -s .000001 -W 1024 -H 1024 -m 1000 -n # (cse3320.org) </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2242,18 +2896,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$50:$B$51</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>mandel -x 0.2869325 -y 0.0142905 -s .000001 -W 1024 -H 1024 -m 1000 -n # (cse3320.org)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>execution time (usec)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>execution time / # threads</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2473,6 +3116,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2538,6 +3236,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>execution time (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5996,16 +6749,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6033,15 +6786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6068,16 +6821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6105,15 +6858,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6141,15 +6894,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6176,16 +6929,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6512,8 +7265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6B529B-3497-4D5C-A57C-38E835018BEA}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>